<commit_message>
throw exception in import excel
</commit_message>
<xml_diff>
--- a/error.xlsx
+++ b/error.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26623"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" revIDLastSave="17" xr10:uidLastSave="{2AAAC5C0-F687-4732-91C0-2689D84A7B61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoant\OneDrive\Documents\thuctapsaurv1\test_excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="105"/>
+    <workbookView windowHeight="9192" windowWidth="23040" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
     <sheet name="error" r:id="rId5" sheetId="2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,12 +41,6 @@
     <t>Nguyen Van Q</t>
   </si>
   <si>
-    <t>qnguyengmail.com</t>
-  </si>
-  <si>
-    <t>0379999999</t>
-  </si>
-  <si>
     <t>89f1a18f-9497-430c-9a9f-be1bb097218c</t>
   </si>
   <si>
@@ -58,24 +56,30 @@
     <t>Nguyen Van W</t>
   </si>
   <si>
-    <t>wnguyen@gmail.com</t>
-  </si>
-  <si>
     <t>0380000000</t>
   </si>
   <si>
+    <t>qnguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>wnguyengmail.com</t>
+  </si>
+  <si>
+    <t>379999999</t>
+  </si>
+  <si>
+    <t>[phone=Not valid!, Town=Not found!, Code=This field must not be duplicate!, District=Not found!, Province=Not found!]</t>
+  </si>
+  <si>
     <t>[Town=Not found!, Code=This field must not be duplicate!, District=Not found!, email=Not valid!, Province=Not found!]</t>
-  </si>
-  <si>
-    <t>[Town=Not found!, Code=This field must not be duplicate!, District=Not found!, Province=Not found!]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -431,25 +435,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.28515625" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125" collapsed="false"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="3.28515625" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="37.7109375" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="38.85546875" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="39.140625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="3.33203125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.6640625" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="38.88671875" collapsed="false"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="39.109375" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,80 +461,80 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1">
         <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C1" xr:uid="{0D78E5BC-2CD7-473B-B4BC-C3B1F4D34C88}"/>
-    <hyperlink display="qnguyen@gmail.com" r:id="rId2" ref="C2" xr:uid="{1E7A3BF4-561A-48D1-A779-1D3175BFC367}"/>
-    <hyperlink r:id="rId3" ref="C2" xr:uid="{7499A539-4962-4B82-8881-399D55956A81}"/>
+    <hyperlink r:id="rId1" ref="C1"/>
+    <hyperlink display="qnguyen@gmail.com" r:id="rId2" ref="C2"/>
+    <hyperlink display="wnguyen@gmail.com" r:id="rId3" ref="C2"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="3.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="38.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="3.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="38.88671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="39.109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -538,51 +542,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1">
         <v>20</v>
       </c>
       <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2">
         <v>20</v>
       </c>
       <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
         <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>6</v>
       </c>
       <c r="I2" t="s">
         <v>12</v>
@@ -590,9 +594,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="C1" xr:uid="{0D78E5BC-2CD7-473B-B4BC-C3B1F4D34C88}"/>
-    <hyperlink display="qnguyen@gmail.com" r:id="rId2" ref="C2" xr:uid="{1E7A3BF4-561A-48D1-A779-1D3175BFC367}"/>
-    <hyperlink r:id="rId3" ref="C2" xr:uid="{7499A539-4962-4B82-8881-399D55956A81}"/>
+    <hyperlink r:id="rId1" ref="C1"/>
+    <hyperlink display="qnguyen@gmail.com" r:id="rId2" ref="C2"/>
+    <hyperlink display="wnguyen@gmail.com" r:id="rId3" ref="C2"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>